<commit_message>
[Excel Config] Update Excel Config File
</commit_message>
<xml_diff>
--- a/tools/misc/prepare_framework_v2_config.xlsx
+++ b/tools/misc/prepare_framework_v2_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4F92AC-494E-4A3C-A98B-5484E57A4E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F55D92-374A-4EEE-B7A9-8B5E02EADA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{456AA15C-9F04-477A-B891-F9D422524496}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>urn_root</t>
   </si>
@@ -192,9 +192,6 @@
     <t>If you use it, you MUST also define a non-empty "implementation_groups" list (see example below).</t>
   </si>
   <si>
-    <t>This sheet is only required if you use "implementation_groups_sheet_base_name"</t>
-  </si>
-  <si>
     <t>Must contain only letters, digits, dashes (-), underscores (_) or dots (.) — no special chars.</t>
   </si>
   <si>
@@ -211,10 +208,6 @@
   </si>
   <si>
     <t>Use this sheet if you wish to have an additional language</t>
-  </si>
-  <si>
-    <t>Use this sheet if you wish to have an additional language for implementation groups
-This sheet is only required if you use "implementation_groups_sheet_base_name"</t>
   </si>
   <si>
     <t>Prepare Framework V2 Configuration File</t>
@@ -265,9 +258,6 @@
     <t>YELLOW CELL</t>
   </si>
   <si>
-    <t>About sheets :</t>
-  </si>
-  <si>
     <t>About cell colors :</t>
   </si>
   <si>
@@ -482,12 +472,65 @@
   <si>
     <t>Most cells already contain pre-filled values. These are simply example values, all of which can be modified or deleted depending on the cell.</t>
   </si>
+  <si>
+    <t>This sheet can only be used if you use "implementation_groups_sheet_base_name"</t>
+  </si>
+  <si>
+    <t>Use this sheet if you wish to have an additional language for implementation groups
+This sheet can only be used if you use "implementation_groups_sheet_base_name"</t>
+  </si>
+  <si>
+    <t>About sheets colors :</t>
+  </si>
+  <si>
+    <t>About sheets types :</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>#imp_grp</t>
+  </si>
+  <si>
+    <t>#base_xx</t>
+  </si>
+  <si>
+    <t>#imp_grp_xx</t>
+  </si>
+  <si>
+    <t>Main sheet</t>
+  </si>
+  <si>
+    <t>Main sheet containing all the strict minimum values in ordrer to create a framework</t>
+  </si>
+  <si>
+    <t>Optional sheet to add an additionnal language to certain values in the "base" sheet</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Optional sheet for creating implementation groups. The table on the left is the one to fill in. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tip: If you want to add implementation groups to the framework but don't know them yet, you can create an empty implementation groups sheet in the output framework by removing the "#" from "implementation_groups_sheet_base_name" in "base" and leaving the sheet name "#imp_grp" as is.</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional sheet to add an additionnal language to certain values in the "imp_grp" sheet. A value put in the "ref_id" column of this sheet must also exist int the "ref_id" column of the "imp_grp" sheet.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,24 +572,6 @@
       <b/>
       <sz val="48"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -616,8 +641,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +719,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -860,7 +922,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -886,122 +947,148 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1346,10 +1433,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,269 +1448,371 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="45"/>
+    </row>
+    <row r="3" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="30"/>
+    </row>
+    <row r="5" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34"/>
-    </row>
-    <row r="2" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="30"/>
+    </row>
+    <row r="6" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="30"/>
+    </row>
+    <row r="7" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="54"/>
+    </row>
+    <row r="8" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57"/>
+    </row>
+    <row r="9" spans="1:13" ht="47.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
+    </row>
+    <row r="10" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
+    </row>
+    <row r="11" spans="1:13" ht="40.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="63"/>
+    </row>
+    <row r="12" spans="1:13" s="7" customFormat="1" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-    </row>
-    <row r="3" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+    </row>
+    <row r="13" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
+    </row>
+    <row r="15" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
+    </row>
+    <row r="16" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="40"/>
-    </row>
-    <row r="4" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="46"/>
-    </row>
-    <row r="6" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="46"/>
-    </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="58" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="30"/>
+    </row>
+    <row r="17" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="30"/>
+    </row>
+    <row r="18" spans="1:13" s="7" customFormat="1" ht="17.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-    </row>
-    <row r="8" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="40"/>
-    </row>
-    <row r="9" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="46"/>
-    </row>
-    <row r="10" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="46"/>
-    </row>
-    <row r="11" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="46"/>
-    </row>
-    <row r="12" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="46"/>
-    </row>
-    <row r="13" spans="1:13" s="7" customFormat="1" ht="17.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:M13"/>
-    <mergeCell ref="A8:M8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="G9:M9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:M11"/>
+  <mergeCells count="31">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:M11"/>
+    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C9:M9"/>
+    <mergeCell ref="C8:M8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A7:M7"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:M12"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:M18"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="G14:M14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="G15:M15"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="G16:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1634,141 +1823,151 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="121.44140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>40</v>
-      </c>
+    <row r="1" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1790,47 +1989,47 @@
     <col min="1" max="1" width="11.5546875" style="5"/>
     <col min="2" max="2" width="22.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="2" style="11" customWidth="1"/>
+    <col min="4" max="4" width="2" style="10" customWidth="1"/>
     <col min="5" max="5" width="72.6640625" style="7" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" style="7" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="E1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="E1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>69</v>
+      <c r="G2" s="12" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1880,7 +2079,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,20 +2090,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A1" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1947,7 +2146,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,47 +2154,46 @@
     <col min="1" max="1" width="11.5546875" style="2"/>
     <col min="2" max="2" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="2.109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="73.88671875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="73.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="E1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>69</v>
+      <c r="G2" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Excel Config] Add Sheet Protection to Excel Config File
Only cells intended to be modified can be. This will prevent users from accidentaly modifying a cell that should't be.
</commit_message>
<xml_diff>
--- a/tools/misc/prepare_framework_v2_config.xlsx
+++ b/tools/misc/prepare_framework_v2_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C1BBBC-03CE-4FF9-9F84-0D9215089AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989B7E7D-EA67-4161-8C97-C42939E38F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{456AA15C-9F04-477A-B891-F9D422524496}"/>
   </bookViews>
@@ -952,17 +952,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1004,9 +995,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1016,6 +1004,90 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1025,51 +1097,6 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1079,41 +1106,14 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1133,17 +1133,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1502,377 +1506,360 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="47"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="2" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
     </row>
     <row r="3" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="35"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="33" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="35"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="33" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="35"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="30"/>
     </row>
     <row r="7" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
     </row>
     <row r="8" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="33" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="35"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="30"/>
     </row>
     <row r="9" spans="1:13" ht="47.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="54" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
     </row>
     <row r="10" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="33" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="35"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
     </row>
     <row r="11" spans="1:13" ht="40.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="51" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="53"/>
-    </row>
-    <row r="12" spans="1:13" s="7" customFormat="1" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="48"/>
+      <c r="C12" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
     </row>
     <row r="13" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
     </row>
     <row r="14" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33" t="s">
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="35"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="33" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="35"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
     </row>
     <row r="16" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="33" t="s">
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="35"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="30"/>
     </row>
     <row r="17" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="33" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="35"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="30"/>
     </row>
     <row r="18" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="33" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="35"/>
-    </row>
-    <row r="19" spans="1:13" s="7" customFormat="1" ht="17.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="24" t="s">
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="30"/>
+    </row>
+    <row r="19" spans="1:13" s="4" customFormat="1" ht="17.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
     </row>
     <row r="20" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="33">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:M11"/>
-    <mergeCell ref="C10:M10"/>
-    <mergeCell ref="C9:M9"/>
-    <mergeCell ref="C8:M8"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="A7:M7"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:M12"/>
     <mergeCell ref="A19:B19"/>
@@ -1888,6 +1875,24 @@
     <mergeCell ref="G16:M16"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="G18:M18"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:M11"/>
+    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C9:M9"/>
+    <mergeCell ref="C8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1919,127 +1924,128 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -2062,13 +2068,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="5"/>
-    <col min="2" max="2" width="22.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="2" style="10" customWidth="1"/>
-    <col min="5" max="5" width="72.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="64"/>
+    <col min="2" max="2" width="22.6640625" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="64" customWidth="1"/>
+    <col min="4" max="4" width="2" style="7" customWidth="1"/>
+    <col min="5" max="5" width="72.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -2077,68 +2083,69 @@
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="64" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="64" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="64" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -2155,7 +2162,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2173,39 +2180,40 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -2227,10 +2235,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="2"/>
-    <col min="2" max="2" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="2.109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="66"/>
+    <col min="2" max="2" width="22.6640625" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5546875" style="66" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="73.88671875" customWidth="1"/>
     <col min="6" max="6" width="9.77734375" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" customWidth="1"/>
@@ -2242,68 +2250,69 @@
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="64" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="64" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="64"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>

</xml_diff>